<commit_message>
feat: Recipe DB, Excel 추가
</commit_message>
<xml_diff>
--- a/Assets/9. RawData/ItemDBSheet.xlsx
+++ b/Assets/9. RawData/ItemDBSheet.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity Work\Project_O\Assets\9. RawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA870ADB-1C37-4D8B-877E-28A507244D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA123E3D-369C-49CF-8CE9-9B799144CEDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B5831765-89E1-4774-865E-255ADA0983F3}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{B5831765-89E1-4774-865E-255ADA0983F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Items!$A$1:$G$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Items!$A$1:$G$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
   <si>
     <t>Material</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -170,6 +170,55 @@
   </si>
   <si>
     <t>Items/Flower_Item</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>에메랄드 에센스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>루비 물약</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>별가루 캔디</t>
+  </si>
+  <si>
+    <t>핑크 프로틴 쉐이크</t>
+  </si>
+  <si>
+    <t>오스틴-코기 포도잼</t>
+  </si>
+  <si>
+    <t>민트 스톡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Combination</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>에메랄드 빛의 에센스. 향긋한 허브향이 나는 꾸덕한 느낌의 향신료이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>루비 색의 물약. 매콤하면서 강렬한 향이 나는 물약으로 남자들이 주로 많이 찾는다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>밤하늘의 별을 따온 듯한 모습의 사탕. 입 안에서 달달한 폭죽이 터지면서 먹은 이들의 행복을 찾아준다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>헬스인들을 위한 분홍빛의 프로틴 쉐이크. 매일 아침 챙겨 먹으면 건강해 질 것 같다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>젤리같은 느낌의 포도잼. 품격있는 오스틴 포도의 맛과 중독성 있는 향이 나는 맛있는 잼이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>민트의 향이 나는 향신료. 풍부한 감칠맛과 향긋한 민트향으로 주부들에게 인기가 많다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -177,7 +226,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,6 +258,12 @@
       <charset val="129"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1D1C1D"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -232,7 +287,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -242,11 +297,55 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -381,44 +480,6 @@
         <scheme val="major"/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="major"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="major"/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -433,16 +494,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3610AA72-8126-4404-8099-054FD17C5423}" name="표1" displayName="표1" ref="A1:G13" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:G13" xr:uid="{B573BBAF-44EB-4B03-AB00-C2B37A8359B3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3610AA72-8126-4404-8099-054FD17C5423}" name="표1" displayName="표1" ref="A1:G19" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="A1:G19" xr:uid="{B573BBAF-44EB-4B03-AB00-C2B37A8359B3}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{988EB226-54C8-4485-9C8D-F94B75018D07}" name="_id" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{DF7F6797-40AC-4B35-B522-E00B7AB41D0B}" name="_name" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{DF703AED-9AAF-409B-95F6-FABE5503A0C4}" name="_description" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{283AE3DC-F666-47FD-80E3-D9745A5BD656}" name="_type" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{7E2371E4-1052-49E1-A832-F48F1294B969}" name="_stack" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{2543C223-8884-4C65-A940-A8036737F5DB}" name="_price" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{4FC0C1D8-F262-46A6-A3C0-B53DAEF94F3B}" name="_spritePath" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{988EB226-54C8-4485-9C8D-F94B75018D07}" name="_id" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{DF7F6797-40AC-4B35-B522-E00B7AB41D0B}" name="_name" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{DF703AED-9AAF-409B-95F6-FABE5503A0C4}" name="_description" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{283AE3DC-F666-47FD-80E3-D9745A5BD656}" name="_type" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{7E2371E4-1052-49E1-A832-F48F1294B969}" name="_stack" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{2543C223-8884-4C65-A940-A8036737F5DB}" name="_price" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{4FC0C1D8-F262-46A6-A3C0-B53DAEF94F3B}" name="_spritePath" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -745,10 +806,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B573BBAF-44EB-4B03-AB00-C2B37A8359B3}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -756,7 +817,7 @@
     <col min="1" max="1" width="8.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="91.75" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1"/>
     <col min="6" max="6" width="8.75" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="41.75" style="1" bestFit="1" customWidth="1"/>
@@ -995,7 +1056,124 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C14" s="2"/>
+      <c r="A14" s="1">
+        <v>2001001</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="1">
+        <v>20</v>
+      </c>
+      <c r="F14" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>2001002</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="1">
+        <v>20</v>
+      </c>
+      <c r="F15" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>2001003</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="1">
+        <v>20</v>
+      </c>
+      <c r="F16" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>2001004</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="1">
+        <v>20</v>
+      </c>
+      <c r="F17" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>2001005</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="1">
+        <v>20</v>
+      </c>
+      <c r="F18" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>2001006</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="1">
+        <v>20</v>
+      </c>
+      <c r="F19" s="1">
+        <v>600</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
fix: item엑셀 id 값 변경
</commit_message>
<xml_diff>
--- a/Assets/9. RawData/ItemDBSheet.xlsx
+++ b/Assets/9. RawData/ItemDBSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity Work\Project_O\Assets\9. RawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA123E3D-369C-49CF-8CE9-9B799144CEDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F638CB-4D29-4A1D-8038-D99FA49DC496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{B5831765-89E1-4774-865E-255ADA0983F3}"/>
+    <workbookView xWindow="2550" yWindow="525" windowWidth="22500" windowHeight="14100" xr2:uid="{B5831765-89E1-4774-865E-255ADA0983F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
@@ -396,12 +396,13 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF1D1C1D"/>
         <name val="맑은 고딕"/>
         <family val="3"/>
         <charset val="129"/>
         <scheme val="major"/>
       </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -434,13 +435,12 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color rgb="FF1D1C1D"/>
+        <color theme="1"/>
         <name val="맑은 고딕"/>
         <family val="3"/>
         <charset val="129"/>
         <scheme val="major"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -494,16 +494,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3610AA72-8126-4404-8099-054FD17C5423}" name="표1" displayName="표1" ref="A1:G19" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3610AA72-8126-4404-8099-054FD17C5423}" name="표1" displayName="표1" ref="A1:G19" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:G19" xr:uid="{B573BBAF-44EB-4B03-AB00-C2B37A8359B3}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{988EB226-54C8-4485-9C8D-F94B75018D07}" name="_id" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{DF7F6797-40AC-4B35-B522-E00B7AB41D0B}" name="_name" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{DF703AED-9AAF-409B-95F6-FABE5503A0C4}" name="_description" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{283AE3DC-F666-47FD-80E3-D9745A5BD656}" name="_type" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{7E2371E4-1052-49E1-A832-F48F1294B969}" name="_stack" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{2543C223-8884-4C65-A940-A8036737F5DB}" name="_price" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{4FC0C1D8-F262-46A6-A3C0-B53DAEF94F3B}" name="_spritePath" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{988EB226-54C8-4485-9C8D-F94B75018D07}" name="_id" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{DF7F6797-40AC-4B35-B522-E00B7AB41D0B}" name="_name" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{DF703AED-9AAF-409B-95F6-FABE5503A0C4}" name="_description" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{283AE3DC-F666-47FD-80E3-D9745A5BD656}" name="_type" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{7E2371E4-1052-49E1-A832-F48F1294B969}" name="_stack" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{2543C223-8884-4C65-A940-A8036737F5DB}" name="_price" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{4FC0C1D8-F262-46A6-A3C0-B53DAEF94F3B}" name="_spritePath" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -809,12 +809,12 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A14" sqref="A14:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="91.75" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.875" style="1" bestFit="1" customWidth="1"/>
@@ -850,7 +850,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>1001001</v>
+        <v>10010001</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -870,7 +870,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>1001002</v>
+        <v>10010002</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -887,7 +887,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>1001003</v>
+        <v>10010003</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
@@ -904,7 +904,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>1001004</v>
+        <v>10010004</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
@@ -921,7 +921,7 @@
     </row>
     <row r="6" spans="1:7" ht="33" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>1001005</v>
+        <v>10010005</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
@@ -938,7 +938,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>1001006</v>
+        <v>10010006</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>6</v>
@@ -955,7 +955,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>1002001</v>
+        <v>10020001</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
@@ -972,7 +972,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>1002002</v>
+        <v>10020002</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>8</v>
@@ -989,7 +989,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>1002003</v>
+        <v>10020003</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
@@ -1006,7 +1006,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>1002004</v>
+        <v>10020004</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>10</v>
@@ -1023,7 +1023,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>1002005</v>
+        <v>10020005</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>11</v>
@@ -1040,7 +1040,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>1002006</v>
+        <v>10020006</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>12</v>
@@ -1057,7 +1057,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>2001001</v>
+        <v>20010001</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>33</v>
@@ -1077,7 +1077,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>2001002</v>
+        <v>20010002</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>34</v>
@@ -1097,7 +1097,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>2001003</v>
+        <v>20010003</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>35</v>
@@ -1117,7 +1117,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>2001004</v>
+        <v>20010004</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>36</v>
@@ -1137,7 +1137,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>2001005</v>
+        <v>20010005</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>37</v>
@@ -1157,7 +1157,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>2001006</v>
+        <v>20010006</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
feat: Invetory Script 추가, Resources 폴더 이동
</commit_message>
<xml_diff>
--- a/Assets/9. RawData/ItemDBSheet.xlsx
+++ b/Assets/9. RawData/ItemDBSheet.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity Work\Project_O\Assets\9. RawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F638CB-4D29-4A1D-8038-D99FA49DC496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B062C29-FEE2-4AFD-96D5-1AAFBCD5A785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2550" yWindow="525" windowWidth="22500" windowHeight="14100" xr2:uid="{B5831765-89E1-4774-865E-255ADA0983F3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B5831765-89E1-4774-865E-255ADA0983F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Items!$A$1:$G$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Items!$A$1:$H$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
   <si>
     <t>Material</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -219,6 +219,10 @@
   </si>
   <si>
     <t>민트의 향이 나는 향신료. 풍부한 감칠맛과 향긋한 민트향으로 주부들에게 인기가 많다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_maxstack</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -307,7 +311,26 @@
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -494,14 +517,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3610AA72-8126-4404-8099-054FD17C5423}" name="표1" displayName="표1" ref="A1:G19" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:G19" xr:uid="{B573BBAF-44EB-4B03-AB00-C2B37A8359B3}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{988EB226-54C8-4485-9C8D-F94B75018D07}" name="_id" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{DF7F6797-40AC-4B35-B522-E00B7AB41D0B}" name="_name" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{DF703AED-9AAF-409B-95F6-FABE5503A0C4}" name="_description" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{283AE3DC-F666-47FD-80E3-D9745A5BD656}" name="_type" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{7E2371E4-1052-49E1-A832-F48F1294B969}" name="_stack" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3610AA72-8126-4404-8099-054FD17C5423}" name="표1" displayName="표1" ref="A1:H19" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:H19" xr:uid="{B573BBAF-44EB-4B03-AB00-C2B37A8359B3}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{988EB226-54C8-4485-9C8D-F94B75018D07}" name="_id" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{DF7F6797-40AC-4B35-B522-E00B7AB41D0B}" name="_name" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{DF703AED-9AAF-409B-95F6-FABE5503A0C4}" name="_description" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{283AE3DC-F666-47FD-80E3-D9745A5BD656}" name="_type" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{31D0B092-3C0B-4AAB-B89E-6F764FCB8F16}" name="_stack" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{7E2371E4-1052-49E1-A832-F48F1294B969}" name="_maxstack" dataDxfId="2"/>
     <tableColumn id="6" xr3:uid="{2543C223-8884-4C65-A940-A8036737F5DB}" name="_price" dataDxfId="1"/>
     <tableColumn id="7" xr3:uid="{4FC0C1D8-F262-46A6-A3C0-B53DAEF94F3B}" name="_spritePath" dataDxfId="0"/>
   </tableColumns>
@@ -806,10 +830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B573BBAF-44EB-4B03-AB00-C2B37A8359B3}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:A19"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -819,13 +843,13 @@
     <col min="3" max="3" width="91.75" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1"/>
-    <col min="6" max="6" width="8.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -842,13 +866,16 @@
         <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>10010001</v>
       </c>
@@ -862,13 +889,16 @@
         <v>0</v>
       </c>
       <c r="E2" s="1">
-        <v>20</v>
-      </c>
-      <c r="G2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>10010002</v>
       </c>
@@ -882,10 +912,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>10010003</v>
       </c>
@@ -899,10 +932,13 @@
         <v>0</v>
       </c>
       <c r="E4" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>10010004</v>
       </c>
@@ -916,10 +952,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>10010005</v>
       </c>
@@ -933,10 +972,13 @@
         <v>0</v>
       </c>
       <c r="E6" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>10010006</v>
       </c>
@@ -950,10 +992,13 @@
         <v>0</v>
       </c>
       <c r="E7" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>10020001</v>
       </c>
@@ -967,10 +1012,13 @@
         <v>0</v>
       </c>
       <c r="E8" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>10020002</v>
       </c>
@@ -984,10 +1032,13 @@
         <v>0</v>
       </c>
       <c r="E9" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>10020003</v>
       </c>
@@ -1001,10 +1052,13 @@
         <v>0</v>
       </c>
       <c r="E10" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10020004</v>
       </c>
@@ -1018,10 +1072,13 @@
         <v>0</v>
       </c>
       <c r="E11" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10020005</v>
       </c>
@@ -1035,10 +1092,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>10020006</v>
       </c>
@@ -1052,10 +1112,13 @@
         <v>0</v>
       </c>
       <c r="E13" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>20010001</v>
       </c>
@@ -1069,13 +1132,16 @@
         <v>39</v>
       </c>
       <c r="E14" s="1">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="F14" s="1">
+        <v>20</v>
+      </c>
+      <c r="G14" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>20010002</v>
       </c>
@@ -1089,13 +1155,16 @@
         <v>39</v>
       </c>
       <c r="E15" s="1">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="F15" s="1">
+        <v>20</v>
+      </c>
+      <c r="G15" s="1">
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>20010003</v>
       </c>
@@ -1109,13 +1178,16 @@
         <v>39</v>
       </c>
       <c r="E16" s="1">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="F16" s="1">
+        <v>20</v>
+      </c>
+      <c r="G16" s="1">
         <v>300</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>20010004</v>
       </c>
@@ -1129,13 +1201,16 @@
         <v>39</v>
       </c>
       <c r="E17" s="1">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="F17" s="1">
+        <v>20</v>
+      </c>
+      <c r="G17" s="1">
         <v>400</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>20010005</v>
       </c>
@@ -1149,13 +1224,16 @@
         <v>39</v>
       </c>
       <c r="E18" s="1">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="F18" s="1">
+        <v>20</v>
+      </c>
+      <c r="G18" s="1">
         <v>500</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>20010006</v>
       </c>
@@ -1169,9 +1247,12 @@
         <v>39</v>
       </c>
       <c r="E19" s="1">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="F19" s="1">
+        <v>20</v>
+      </c>
+      <c r="G19" s="1">
         <v>600</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: Inventory 스크립트 변경
</commit_message>
<xml_diff>
--- a/Assets/9. RawData/ItemDBSheet.xlsx
+++ b/Assets/9. RawData/ItemDBSheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\STIKA\Unity\Project_O\Assets\9. RawData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity Work\Project_O\Assets\9. RawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A691B0E3-FCC3-4488-A626-18227AF14FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61432837-9F6F-42AF-9D68-C346CF19676B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B5831765-89E1-4774-865E-255ADA0983F3}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="77">
   <si>
     <t>Material</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -259,6 +259,90 @@
   </si>
   <si>
     <t>Material</t>
+  </si>
+  <si>
+    <t>Items/CandyTree_Item</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Items/Man-EatingFlower_Item</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Items/Grape_Item</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Items/Herb_Item</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Items/Mushroom_Item</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Items/Turtle_Item</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Items/Grasshopper_Item</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Items/Firelizard_Item</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Items/Corgi_Item</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Items/Kirby_Item</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CombineItems/Emerald_Potion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CombineItems/Ruby_Potion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CombineItems/Star_Candy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CombineItems/Pink_Protain_Shake</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CombineItems/Ostin-Corgi_Jam</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CombineItems/Mint_Stock</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Items/FlySalamander_Item</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Items/LittleGlass_Item</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Items/BigGlass_Item</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Items/JamGlass_Item</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Items/CandyWrap_Item</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -871,7 +955,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -883,7 +967,7 @@
     <col min="5" max="5" width="9" style="1"/>
     <col min="6" max="6" width="12.75" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.25" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -955,6 +1039,9 @@
       <c r="F3" s="1">
         <v>20</v>
       </c>
+      <c r="H3" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -975,6 +1062,9 @@
       <c r="F4" s="1">
         <v>20</v>
       </c>
+      <c r="H4" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -995,6 +1085,9 @@
       <c r="F5" s="1">
         <v>20</v>
       </c>
+      <c r="H5" s="1" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -1015,6 +1108,9 @@
       <c r="F6" s="1">
         <v>20</v>
       </c>
+      <c r="H6" s="1" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -1035,6 +1131,9 @@
       <c r="F7" s="1">
         <v>20</v>
       </c>
+      <c r="H7" s="1" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -1055,6 +1154,9 @@
       <c r="F8" s="1">
         <v>20</v>
       </c>
+      <c r="H8" s="1" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -1075,6 +1177,9 @@
       <c r="F9" s="1">
         <v>20</v>
       </c>
+      <c r="H9" s="1" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -1095,6 +1200,9 @@
       <c r="F10" s="1">
         <v>20</v>
       </c>
+      <c r="H10" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -1115,6 +1223,9 @@
       <c r="F11" s="1">
         <v>20</v>
       </c>
+      <c r="H11" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -1135,6 +1246,9 @@
       <c r="F12" s="1">
         <v>20</v>
       </c>
+      <c r="H12" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -1155,6 +1269,9 @@
       <c r="F13" s="1">
         <v>20</v>
       </c>
+      <c r="H13" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -1178,6 +1295,9 @@
       <c r="G14" s="1">
         <v>20</v>
       </c>
+      <c r="H14" s="1" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
@@ -1201,6 +1321,9 @@
       <c r="G15" s="1">
         <v>30</v>
       </c>
+      <c r="H15" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
@@ -1224,8 +1347,11 @@
       <c r="G16" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>10030004</v>
       </c>
@@ -1247,8 +1373,11 @@
       <c r="G17" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>20010001</v>
       </c>
@@ -1270,8 +1399,11 @@
       <c r="G18" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H18" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>20010002</v>
       </c>
@@ -1293,8 +1425,11 @@
       <c r="G19" s="1">
         <v>200</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H19" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>20010003</v>
       </c>
@@ -1316,8 +1451,11 @@
       <c r="G20" s="1">
         <v>300</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H20" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20010004</v>
       </c>
@@ -1339,8 +1477,11 @@
       <c r="G21" s="1">
         <v>400</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H21" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>20010005</v>
       </c>
@@ -1362,8 +1503,11 @@
       <c r="G22" s="1">
         <v>500</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H22" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>20010006</v>
       </c>
@@ -1384,6 +1528,9 @@
       </c>
       <c r="G23" s="1">
         <v>600</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>